<commit_message>
Sesión 4 - Ejercicio 26
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -57,9 +57,6 @@
     <t>Erika</t>
   </si>
   <si>
-    <t>Fatima</t>
-  </si>
-  <si>
     <t>Gaby</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>Muj.</t>
   </si>
   <si>
-    <t>Femenino</t>
-  </si>
-  <si>
     <t>Fem.</t>
   </si>
   <si>
@@ -103,6 +97,12 @@
   </si>
   <si>
     <t>Licenciatura</t>
+  </si>
+  <si>
+    <t>Fabian</t>
+  </si>
+  <si>
+    <t>masculino</t>
   </si>
 </sst>
 </file>
@@ -570,8 +570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="290" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="286" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -598,10 +598,10 @@
         <v>12</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
@@ -612,10 +612,10 @@
         <v>15</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.2">
@@ -626,10 +626,10 @@
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.2">
@@ -640,10 +640,10 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.2">
@@ -654,38 +654,38 @@
         <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C12">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13">
         <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>